<commit_message>
week 7 parsed to csv's
</commit_message>
<xml_diff>
--- a/data/Experiment/Raw/Spreadsheets/Physiology_09052025.xlsx
+++ b/data/Experiment/Raw/Spreadsheets/Physiology_09052025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernbromley/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5911ECF4-EEE9-9F4C-A5F2-760D026990C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD45A5E-D341-354D-9429-0B32B3B040AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="10000" windowHeight="17160" activeTab="1" xr2:uid="{CA551DF1-0ED1-674A-8F89-05216640288A}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="10000" windowHeight="17160" xr2:uid="{CA551DF1-0ED1-674A-8F89-05216640288A}"/>
   </bookViews>
   <sheets>
     <sheet name="PIFL" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
   <si>
     <t>TreeID</t>
   </si>
@@ -163,9 +163,6 @@
   </si>
   <si>
     <t>Conductance_mmol_m2s</t>
-  </si>
-  <si>
-    <t>VWC_perc</t>
   </si>
 </sst>
 </file>
@@ -559,247 +556,183 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6B18CAA-D5E2-8F4D-8617-88F8364D5DB9}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="187" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="187" workbookViewId="0">
+      <selection activeCell="C8" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>41</v>
       </c>
-      <c r="C1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2">
         <v>203.1</v>
       </c>
-      <c r="C2">
-        <v>13.7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
         <v>227.8</v>
       </c>
-      <c r="C3">
-        <v>6.8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B4">
         <v>237.4</v>
       </c>
-      <c r="C4">
-        <v>15.4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B5">
         <v>162.30000000000001</v>
       </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B6">
         <v>334.9</v>
       </c>
-      <c r="C6">
-        <v>12.7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B7">
         <v>310.2</v>
       </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B8">
         <v>358.3</v>
       </c>
-      <c r="C8">
-        <v>13.1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B9">
         <v>180.3</v>
       </c>
-      <c r="C9">
-        <v>7.7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B10">
         <v>306.60000000000002</v>
       </c>
-      <c r="C10">
-        <v>11.1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B11">
         <v>193.5</v>
       </c>
-      <c r="C11">
-        <v>7.4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B12">
         <v>210.6</v>
       </c>
-      <c r="C12">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B13">
         <v>241.3</v>
       </c>
-      <c r="C13">
-        <v>7.4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B14">
         <v>174.5</v>
       </c>
-      <c r="C14">
-        <v>10.9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B15">
         <v>246.2</v>
       </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B16">
         <v>305.8</v>
       </c>
-      <c r="C16">
-        <v>12.4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B17">
         <v>284.8</v>
       </c>
-      <c r="C17">
-        <v>6.9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B18">
         <v>328.8</v>
       </c>
-      <c r="C18">
-        <v>16.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B19">
         <v>284</v>
       </c>
-      <c r="C19">
-        <v>3.1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B20">
         <v>334</v>
       </c>
-      <c r="C20">
-        <v>9.3000000000000007</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B21">
         <v>169.9</v>
-      </c>
-      <c r="C21">
-        <v>1.2</v>
       </c>
     </row>
   </sheetData>
@@ -809,247 +742,183 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{115E6809-C6E9-4B42-AF0B-D16D811C3B7F}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="168" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView zoomScale="168" workbookViewId="0">
+      <selection activeCell="C7" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>41</v>
       </c>
-      <c r="C1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B2">
         <v>279.10000000000002</v>
       </c>
-      <c r="C2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B3">
         <v>206.5</v>
       </c>
-      <c r="C3">
-        <v>3.2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B4">
         <v>110.7</v>
       </c>
-      <c r="C4">
-        <v>17.3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B5">
         <v>214.4</v>
       </c>
-      <c r="C5">
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B6">
         <v>244.3</v>
       </c>
-      <c r="C6">
-        <v>13.2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B7">
         <v>179.7</v>
       </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B8">
         <v>257.5</v>
       </c>
-      <c r="C8">
-        <v>17.899999999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B9">
         <v>145.30000000000001</v>
       </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B10">
         <v>367.7</v>
       </c>
-      <c r="C10">
-        <v>14.8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B11">
         <v>98.6</v>
       </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B12">
         <v>169.5</v>
       </c>
-      <c r="C12">
-        <v>14.3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B13">
         <v>123</v>
       </c>
-      <c r="C13">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B14">
         <v>361.2</v>
       </c>
-      <c r="C14">
-        <v>14.9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B15">
         <v>140</v>
       </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B16">
         <v>160.6</v>
       </c>
-      <c r="C16">
-        <v>14.1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B17">
         <v>74.8</v>
       </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B18">
         <v>346.6</v>
       </c>
-      <c r="C18">
-        <v>16.8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B19">
         <v>110.7</v>
       </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B20">
         <v>444.2</v>
       </c>
-      <c r="C20">
-        <v>16.5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B21">
         <v>151.19999999999999</v>
-      </c>
-      <c r="C21">
-        <v>0.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>